<commit_message>
ok pour la présentation
</commit_message>
<xml_diff>
--- a/Excel tests/test 3d.xlsx
+++ b/Excel tests/test 3d.xlsx
@@ -25,13 +25,27 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -54,9 +68,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,65 +388,565 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>2</v>
       </c>
       <c r="B1" s="1">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="C3" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C6" s="1">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>4</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>4</v>
+      </c>
+      <c r="B10" s="1">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="C11" s="1">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="C3">
+      <c r="C13" s="1">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>6</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>8</v>
+      </c>
+      <c r="B16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
-        <v>-1</v>
-      </c>
-      <c r="C4">
-        <v>-11</v>
+      <c r="C16" s="1">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>8</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>10</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>10</v>
+      </c>
+      <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>10</v>
+      </c>
+      <c r="B25" s="1">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1">
+        <v>2</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>12</v>
+      </c>
+      <c r="B30" s="1">
+        <v>4</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>14</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>14</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>14</v>
+      </c>
+      <c r="B34" s="1">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>14</v>
+      </c>
+      <c r="B35" s="1">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <v>0</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>16</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>16</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1">
+        <v>2</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>16</v>
+      </c>
+      <c r="B40" s="1">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>18</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>18</v>
+      </c>
+      <c r="B42" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>18</v>
+      </c>
+      <c r="B43" s="1">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0.21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>18</v>
+      </c>
+      <c r="B44" s="1">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>18</v>
+      </c>
+      <c r="B45" s="1">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>20</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>20</v>
+      </c>
+      <c r="B47" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>20</v>
+      </c>
+      <c r="B48" s="1">
+        <v>1</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>20</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>20</v>
+      </c>
+      <c r="B50" s="1">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>